<commit_message>
Elisa notes different from the current work on dose response experiments
</commit_message>
<xml_diff>
--- a/elisa.xlsx
+++ b/elisa.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SwaggyT\Documents\biophysicsresearch\elisa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GrandProf\Downloads\Repos_4cleanup\Repositories_AP7\Active\Elisa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C264049F-1B7E-433F-BBFE-425A9804CFE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B960D9A1-C37D-4D74-9927-092F9858322B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1470" windowWidth="29040" windowHeight="16440" xr2:uid="{922FE556-F4D4-41FE-8239-D3DFC09E4A31}"/>
+    <workbookView xWindow="19107" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{922FE556-F4D4-41FE-8239-D3DFC09E4A31}"/>
   </bookViews>
   <sheets>
     <sheet name="elisaduplicate" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3401,15 +3404,15 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="9.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>5.5412896635160163</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -3493,7 +3496,7 @@
         <v>0.31520000100135803</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>0.4627000093460083</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -3545,7 +3548,7 @@
         <v>0.69010001420974731</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>0.85079997777938843</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>1.0078999996185303</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3623,7 +3626,7 @@
         <v>0.9749000072479248</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3649,7 +3652,7 @@
         <v>2.0439999103546143</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -3675,7 +3678,7 @@
         <v>0.17470000684261322</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>1.0211000442504883</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -3727,7 +3730,7 @@
         <v>1.0784000158309937</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -3753,7 +3756,7 @@
         <v>0.36059999465942383</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3779,7 +3782,7 @@
         <v>0.34670001268386841</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>0.48249998688697815</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3831,7 +3834,7 @@
         <v>0.35870000720024109</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -3857,7 +3860,7 @@
         <v>0.33579999208450317</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -3883,7 +3886,7 @@
         <v>0.40239998698234558</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -3909,7 +3912,7 @@
         <v>0.48809999227523804</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3935,7 +3938,7 @@
         <v>0.42950001358985901</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -3961,7 +3964,7 @@
         <v>0.35109999775886536</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3987,7 +3990,7 @@
         <v>0.35429999232292175</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -4013,7 +4016,7 @@
         <v>0.43489998579025269</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -4039,7 +4042,7 @@
         <v>0.37090000510215759</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -4065,7 +4068,7 @@
         <v>0.35980001091957092</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -4091,7 +4094,7 @@
         <v>0.33349999785423279</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -4117,7 +4120,7 @@
         <v>0.42260000109672502</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -4143,7 +4146,7 @@
         <v>0.37860000133514404</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -4169,7 +4172,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -4195,7 +4198,7 @@
         <v>0.46419999003410339</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -4221,7 +4224,7 @@
         <v>0.49360001087188721</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -4247,7 +4250,7 @@
         <v>0.32069998979568481</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -4273,7 +4276,7 @@
         <v>0.39050000905990601</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -4299,7 +4302,7 @@
         <v>0.34540000557899475</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>0.38699999451637268</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -4351,7 +4354,7 @@
         <v>0.36640000343322754</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -4377,7 +4380,7 @@
         <v>0.3935999870300293</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -4403,7 +4406,7 @@
         <v>0.37209999561309814</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -4429,7 +4432,7 @@
         <v>0.35890001058578491</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4455,7 +4458,7 @@
         <v>0.3564000129699707</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -4481,7 +4484,7 @@
         <v>0.50199997425079346</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -4507,7 +4510,7 @@
         <v>0.38659998774528503</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>0.43209999799728394</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -4559,7 +4562,7 @@
         <v>0.3239000141620636</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -4585,7 +4588,7 @@
         <v>0.36329999566078186</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -4611,7 +4614,7 @@
         <v>0.29170000553131104</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>0</v>
       </c>

</xml_diff>